<commit_message>
Added male youth/junior club records, not run through tool yet
</commit_message>
<xml_diff>
--- a/prev_known.xlsx
+++ b/prev_known.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78878FF8-DA14-4302-B075-D672F17DF6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE737963-A093-4A34-960C-57D003086F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="2790" yWindow="3525" windowWidth="25515" windowHeight="16755" activeTab="3" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="other_known" sheetId="2" r:id="rId1"/>
     <sheet name="C&amp;C_2022_overall" sheetId="1" r:id="rId2"/>
     <sheet name="C&amp;C_2022_ag_female" sheetId="3" r:id="rId3"/>
+    <sheet name="C&amp;C_2022_ag_male" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="sp7.26k_m_all" localSheetId="1">'C&amp;C_2022_overall'!$G$20</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="634">
   <si>
     <r>
       <t>C&amp;C AC Track and Field records  - Overall club records</t>
@@ -1427,6 +1428,600 @@
   </si>
   <si>
     <t>PenU13W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.66 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013 </t>
+  </si>
+  <si>
+    <t>21.07</t>
+  </si>
+  <si>
+    <t>Benjamin Snaith</t>
+  </si>
+  <si>
+    <t>47.14</t>
+  </si>
+  <si>
+    <t>1:48.93</t>
+  </si>
+  <si>
+    <t>Edward Aston</t>
+  </si>
+  <si>
+    <t>3:41.44</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Thomas Keen</t>
+  </si>
+  <si>
+    <t>8:10.2</t>
+  </si>
+  <si>
+    <t>Alex Melloy</t>
+  </si>
+  <si>
+    <t>5000m</t>
+  </si>
+  <si>
+    <t>14:37.51</t>
+  </si>
+  <si>
+    <t>Kieran Wood</t>
+  </si>
+  <si>
+    <t>4:11.5</t>
+  </si>
+  <si>
+    <t>Sprint Hurdles  3’3”</t>
+  </si>
+  <si>
+    <t>13.72</t>
+  </si>
+  <si>
+    <t>Ben Kelk</t>
+  </si>
+  <si>
+    <t>54.2</t>
+  </si>
+  <si>
+    <t>Samuel Clarke</t>
+  </si>
+  <si>
+    <t>5:54.0</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>Graham Tuck</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>Martin Shorten</t>
+  </si>
+  <si>
+    <t>6.80</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>Nigel Coyle</t>
+  </si>
+  <si>
+    <t>15.52</t>
+  </si>
+  <si>
+    <t>Dennis Greene</t>
+  </si>
+  <si>
+    <t>3.30</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>Mark Jennings</t>
+  </si>
+  <si>
+    <t>Shot 6kg</t>
+  </si>
+  <si>
+    <t>14.40</t>
+  </si>
+  <si>
+    <t>Oliver Holway</t>
+  </si>
+  <si>
+    <t>Disc 1.75kg</t>
+  </si>
+  <si>
+    <t>46.83</t>
+  </si>
+  <si>
+    <t>Kristiaan Winkel</t>
+  </si>
+  <si>
+    <t>Discus 2kg</t>
+  </si>
+  <si>
+    <t>42.55</t>
+  </si>
+  <si>
+    <t>2021`</t>
+  </si>
+  <si>
+    <t>Javelin (post 1986)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             (pre 1986)</t>
+  </si>
+  <si>
+    <t>57.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Bradley </t>
+  </si>
+  <si>
+    <t>Bogas Kawalko</t>
+  </si>
+  <si>
+    <t>Ham.6kg</t>
+  </si>
+  <si>
+    <t>47.82</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Oliver Hoad</t>
+  </si>
+  <si>
+    <t>2345 pts</t>
+  </si>
+  <si>
+    <t>Decathlon</t>
+  </si>
+  <si>
+    <t>5790 pts</t>
+  </si>
+  <si>
+    <t>45.1</t>
+  </si>
+  <si>
+    <t>Post 2007</t>
+  </si>
+  <si>
+    <t>J Godden, G Baker,L Crabb ,C Morter</t>
+  </si>
+  <si>
+    <t>3:22.5</t>
+  </si>
+  <si>
+    <t>E Aston, D Potts, D Baker, O Francis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Under 20 men</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under 17 Men </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012 </t>
+  </si>
+  <si>
+    <t>Timothy Cobden</t>
+  </si>
+  <si>
+    <t>Matthew Clements</t>
+  </si>
+  <si>
+    <t>Benedict Kelk</t>
+  </si>
+  <si>
+    <t>Thomas Bridger</t>
+  </si>
+  <si>
+    <t>Innes Murray</t>
+  </si>
+  <si>
+    <t>Deshawn Lascelles</t>
+  </si>
+  <si>
+    <t>C. Hyde</t>
+  </si>
+  <si>
+    <t>John Blackwell</t>
+  </si>
+  <si>
+    <t>David Croxon</t>
+  </si>
+  <si>
+    <t>Jav 700gm</t>
+  </si>
+  <si>
+    <t>2479 pts</t>
+  </si>
+  <si>
+    <t>William Blackwell</t>
+  </si>
+  <si>
+    <t>Octathlon</t>
+  </si>
+  <si>
+    <t>4234 pts</t>
+  </si>
+  <si>
+    <t>Ben Motherwell</t>
+  </si>
+  <si>
+    <t>44.39 s</t>
+  </si>
+  <si>
+    <t>B Snaith, J Ebanks, J Mair, D Doggett</t>
+  </si>
+  <si>
+    <t>21.67</t>
+  </si>
+  <si>
+    <t>47.92</t>
+  </si>
+  <si>
+    <t>1:53.38</t>
+  </si>
+  <si>
+    <t>3:41.4</t>
+  </si>
+  <si>
+    <t>8:22.60</t>
+  </si>
+  <si>
+    <t>12.47</t>
+  </si>
+  <si>
+    <t>54.94</t>
+  </si>
+  <si>
+    <t>4:40.4</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>6.50</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>14.85</t>
+  </si>
+  <si>
+    <t>3.55</t>
+  </si>
+  <si>
+    <t>15.47</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>54.96</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>62.56</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>53.93</t>
+  </si>
+  <si>
+    <t>George Keen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:17.57 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 </t>
+  </si>
+  <si>
+    <t>Under 15 Boys</t>
+  </si>
+  <si>
+    <t>Mathew Clements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1992 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">300m </t>
+  </si>
+  <si>
+    <t>Paul Lambrecht</t>
+  </si>
+  <si>
+    <t>Ewan Taylor</t>
+  </si>
+  <si>
+    <t>Robert Huckle</t>
+  </si>
+  <si>
+    <t>Samuel Boden</t>
+  </si>
+  <si>
+    <t>80m Sprint Hurdles</t>
+  </si>
+  <si>
+    <t>Ben Abbott-gribben</t>
+  </si>
+  <si>
+    <t>Billy White</t>
+  </si>
+  <si>
+    <t>Nick Grundy</t>
+  </si>
+  <si>
+    <t>Morgan Young</t>
+  </si>
+  <si>
+    <t>Luke Shortman</t>
+  </si>
+  <si>
+    <t>2563 Pts</t>
+  </si>
+  <si>
+    <t>David October</t>
+  </si>
+  <si>
+    <t>J.Ebanks,W.Blackwell,J.Mair,B.Snaith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.54 </t>
+  </si>
+  <si>
+    <t>37.8</t>
+  </si>
+  <si>
+    <t>2:01.7</t>
+  </si>
+  <si>
+    <t>4:10.65</t>
+  </si>
+  <si>
+    <t>9:08.5</t>
+  </si>
+  <si>
+    <t>4:43.6</t>
+  </si>
+  <si>
+    <t>10.71</t>
+  </si>
+  <si>
+    <t>1.85</t>
+  </si>
+  <si>
+    <t>6.09</t>
+  </si>
+  <si>
+    <t>12.94</t>
+  </si>
+  <si>
+    <t>2.85</t>
+  </si>
+  <si>
+    <t>13.90</t>
+  </si>
+  <si>
+    <t>43.66</t>
+  </si>
+  <si>
+    <t>55.21</t>
+  </si>
+  <si>
+    <t>50.01</t>
+  </si>
+  <si>
+    <t>46.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under 13 Boys </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G. Dant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1977 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luca McGrath </t>
+  </si>
+  <si>
+    <t>Isaac Morris</t>
+  </si>
+  <si>
+    <t>75m Hurdles</t>
+  </si>
+  <si>
+    <t>Damian Quinn</t>
+  </si>
+  <si>
+    <t>James Cross</t>
+  </si>
+  <si>
+    <t>Shot 3 kg</t>
+  </si>
+  <si>
+    <t>Christopher Springett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jav 400 gm  </t>
+  </si>
+  <si>
+    <t>Frederic Kastner</t>
+  </si>
+  <si>
+    <t>77 pts</t>
+  </si>
+  <si>
+    <t>2012/2013</t>
+  </si>
+  <si>
+    <t>Samuel Clarke/James Richer</t>
+  </si>
+  <si>
+    <t>J Langford, J Markley,B Kelk ,A Morter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.0 </t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>2:13.3</t>
+  </si>
+  <si>
+    <t>4:33.8</t>
+  </si>
+  <si>
+    <t>5:18.6</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>5.06</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>11.40</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.06 </t>
+  </si>
+  <si>
+    <t>35.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under 11 Boys </t>
+  </si>
+  <si>
+    <t>Joseph Ebanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luca Mc.Grath </t>
+  </si>
+  <si>
+    <t>Ollie Waters</t>
+  </si>
+  <si>
+    <t>1:49.4</t>
+  </si>
+  <si>
+    <t>2:38.0</t>
+  </si>
+  <si>
+    <t>5:14.8</t>
+  </si>
+  <si>
+    <t>4.11</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>SP6K</t>
+  </si>
+  <si>
+    <t>DT1.75K</t>
+  </si>
+  <si>
+    <t>PenU20M</t>
+  </si>
+  <si>
+    <t>DT1.25K</t>
+  </si>
+  <si>
+    <t>Assumed weight from modern competition</t>
+  </si>
+  <si>
+    <t>PenU15M</t>
+  </si>
+  <si>
+    <t>80H</t>
+  </si>
+  <si>
+    <t>100H</t>
+  </si>
+  <si>
+    <t>JT700</t>
+  </si>
+  <si>
+    <t>PenU17M</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Guess this is obsolete event now</t>
+  </si>
+  <si>
+    <t>110HU20M</t>
+  </si>
+  <si>
+    <t>Checked Po10 for event</t>
+  </si>
+  <si>
+    <t>Assuming same as modern event for age group</t>
+  </si>
+  <si>
+    <t>HT6K</t>
+  </si>
+  <si>
+    <t>SP5K</t>
+  </si>
+  <si>
+    <t>DT1.5K</t>
   </si>
 </sst>
 </file>
@@ -3325,8 +3920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116B990-5FBC-4F60-A519-6D8AF60704F6}">
   <dimension ref="A2:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5357,4 +5952,1985 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
+  <dimension ref="A2:K88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="19.140625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="10"/>
+    <col min="6" max="6" width="33.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C2" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C5" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C8" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C9" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C10" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C12" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C15" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C17" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C18" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>616</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C23" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C25" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C26" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C30" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C32" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>520</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C33" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>521</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C34" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>539</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C36" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>523</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C37" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C39" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C40" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C41" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>530</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>532</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C44" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>633</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C45" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>624</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C46" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>631</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>625</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C48" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>626</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C49" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C52" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C53" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C55" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C56" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>563</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>549</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C57" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C58" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C59" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C61" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C62" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>551</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C64" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>571</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="K64" s="10" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C65" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>554</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C66" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="K66" s="10" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C67" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C68" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C71" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C72" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C73" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C74" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C75" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>597</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C76" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I76" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C77" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C79" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="K79" s="10" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C80" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>604</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C81" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="H81" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C82" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H82" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="F84" s="10" t="s">
+        <v>606</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="H84" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C85" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C86" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C87" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>613</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F87" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C88" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>614</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="F88" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I88" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Couple of event corrections
</commit_message>
<xml_diff>
--- a/prev_known.xlsx
+++ b/prev_known.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\powerof10-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE737963-A093-4A34-960C-57D003086F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D214273-CCE5-4128-BDA1-AC2CB8DDCE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="3525" windowWidth="25515" windowHeight="16755" activeTab="3" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{59E39808-5DD1-48A0-8CDE-64F5926DA7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="other_known" sheetId="2" r:id="rId1"/>
@@ -1988,12 +1988,6 @@
     <t>PenU15M</t>
   </si>
   <si>
-    <t>80H</t>
-  </si>
-  <si>
-    <t>100H</t>
-  </si>
-  <si>
     <t>JT700</t>
   </si>
   <si>
@@ -2022,6 +2016,12 @@
   </si>
   <si>
     <t>DT1.5K</t>
+  </si>
+  <si>
+    <t>80HU15M</t>
+  </si>
+  <si>
+    <t>100HU17M</t>
   </si>
 </sst>
 </file>
@@ -5958,8 +5958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33EFF66-21E6-4C12-9015-9A2807500A5E}">
   <dimension ref="A2:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6196,7 +6196,7 @@
         <v>454</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>105</v>
@@ -6205,7 +6205,7 @@
         <v>403</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6438,7 +6438,7 @@
         <v>403</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -6478,7 +6478,7 @@
         <v>488</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>105</v>
@@ -6757,7 +6757,7 @@
         <v>502</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>105</v>
@@ -6918,7 +6918,7 @@
         <v>508</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>105</v>
@@ -6927,7 +6927,7 @@
         <v>405</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
@@ -6944,7 +6944,7 @@
         <v>509</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>105</v>
@@ -6953,7 +6953,7 @@
         <v>405</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
@@ -6970,7 +6970,7 @@
         <v>484</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>105</v>
@@ -6993,7 +6993,7 @@
         <v>488</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>105</v>
@@ -7002,7 +7002,7 @@
         <v>405</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
@@ -7019,7 +7019,7 @@
         <v>512</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>105</v>
@@ -7042,7 +7042,7 @@
         <v>515</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>105</v>
@@ -7051,7 +7051,7 @@
         <v>405</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -7255,7 +7255,7 @@
         <v>502</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>105</v>

</xml_diff>